<commit_message>
Create multiple template options
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -1,37 +1,170 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29415"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CB3D011-5043-4AD5-B84B-1559325CEE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>HRName</t>
+  </si>
+  <si>
+    <t>HREmail</t>
+  </si>
+  <si>
+    <t>HRPhone</t>
+  </si>
+  <si>
+    <t>ConfirmationDate</t>
+  </si>
+  <si>
+    <t>SupervisorName</t>
+  </si>
+  <si>
+    <t>OfficeLocation</t>
+  </si>
+  <si>
+    <t>DocumentType</t>
+  </si>
+  <si>
+    <t>Alice Johnson</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>2025-11-01</t>
+  </si>
+  <si>
+    <t>TechNova Inc.</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>john.smith@technova.com</t>
+  </si>
+  <si>
+    <t>+1 555-123-4567</t>
+  </si>
+  <si>
+    <t>2026-02-01</t>
+  </si>
+  <si>
+    <t>Mary Brown</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>probation_confirmation</t>
+  </si>
+  <si>
+    <t>Bob Martinez</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>2025-11-10</t>
+  </si>
+  <si>
+    <t>2026-02-15</t>
+  </si>
+  <si>
+    <t>Emma Davis</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>offer_letter</t>
+  </si>
+  <si>
+    <t>Clara Evans</t>
+  </si>
+  <si>
+    <t>UX Designer</t>
+  </si>
+  <si>
+    <t>2025-12-01</t>
+  </si>
+  <si>
+    <t>2026-03-01</t>
+  </si>
+  <si>
+    <t>James Wilson</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>policy_acknowledgement</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,100 +179,50 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -177,7 +260,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -211,6 +294,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -245,9 +329,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -420,102 +505,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Position</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>StartDate</t>
-        </is>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Alice Smith</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Software Developer</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-10-01</t>
-        </is>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Bob Johnson</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Data Analyst</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-10-05</t>
-        </is>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Charlie Lee</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Project Manager</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2025-10-10</t>
-        </is>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>